<commit_message>
Add Performance section & copypaste data into Timing section
</commit_message>
<xml_diff>
--- a/Performance Testing.xlsx
+++ b/Performance Testing.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Shawn\Documents\GitHub\MatMul\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Charles\Dropbox\CSC 410 Parallel Computing\MatMul\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="10170" windowHeight="11895"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="8820" windowHeight="7410"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -302,12 +302,6 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -322,6 +316,12 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -374,7 +374,7 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US"/>
-              <a:t>Time Comparison - 3 implentations</a:t>
+              <a:t>Time Comparison - 3 implementations</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -4536,629 +4536,629 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView tabSelected="1" topLeftCell="B19" workbookViewId="0">
+      <selection activeCell="Q17" sqref="Q17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="1.28515625" style="4" customWidth="1"/>
-    <col min="2" max="3" width="10" style="4"/>
-    <col min="4" max="4" width="1.28515625" style="4" customWidth="1"/>
-    <col min="5" max="5" width="10" style="4"/>
-    <col min="6" max="6" width="11" style="4" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="1.28515625" style="4" customWidth="1"/>
-    <col min="8" max="8" width="10" style="4"/>
-    <col min="9" max="9" width="11" style="4" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="1.28515625" style="4" customWidth="1"/>
-    <col min="11" max="11" width="10" style="4"/>
-    <col min="12" max="12" width="11" style="4" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="1.28515625" style="4" customWidth="1"/>
-    <col min="14" max="14" width="10" style="4"/>
-    <col min="15" max="15" width="11" style="4" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="1.28515625" style="4" customWidth="1"/>
-    <col min="17" max="16384" width="10" style="4"/>
+    <col min="1" max="1" width="1.28515625" style="2" customWidth="1"/>
+    <col min="2" max="3" width="10" style="2"/>
+    <col min="4" max="4" width="1.28515625" style="2" customWidth="1"/>
+    <col min="5" max="5" width="10" style="2"/>
+    <col min="6" max="6" width="11" style="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="1.28515625" style="2" customWidth="1"/>
+    <col min="8" max="8" width="10" style="2"/>
+    <col min="9" max="9" width="11" style="2" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="1.28515625" style="2" customWidth="1"/>
+    <col min="11" max="11" width="10" style="2"/>
+    <col min="12" max="12" width="11" style="2" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="1.28515625" style="2" customWidth="1"/>
+    <col min="14" max="14" width="10" style="2"/>
+    <col min="15" max="15" width="11" style="2" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="1.28515625" style="2" customWidth="1"/>
+    <col min="17" max="16384" width="10" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1"/>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="3"/>
+      <c r="C1" s="17"/>
       <c r="D1" s="1"/>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="3"/>
+      <c r="F1" s="17"/>
       <c r="G1" s="1"/>
-      <c r="H1" s="2" t="s">
+      <c r="H1" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="I1" s="3"/>
+      <c r="I1" s="17"/>
       <c r="J1" s="1"/>
-      <c r="K1" s="2" t="s">
+      <c r="K1" s="16" t="s">
         <v>5</v>
       </c>
-      <c r="L1" s="3"/>
+      <c r="L1" s="17"/>
       <c r="M1" s="1"/>
-      <c r="N1" s="2" t="s">
+      <c r="N1" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="O1" s="3"/>
+      <c r="O1" s="17"/>
       <c r="P1" s="1"/>
     </row>
     <row r="2" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="5"/>
-      <c r="B2" s="6" t="s">
+      <c r="A2" s="3"/>
+      <c r="B2" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="7" t="s">
+      <c r="C2" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="5"/>
-      <c r="E2" s="6" t="s">
+      <c r="D2" s="3"/>
+      <c r="E2" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="F2" s="7" t="s">
+      <c r="F2" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="G2" s="5"/>
-      <c r="H2" s="6" t="s">
+      <c r="G2" s="3"/>
+      <c r="H2" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="I2" s="7" t="s">
+      <c r="I2" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="J2" s="5"/>
-      <c r="K2" s="6" t="s">
+      <c r="J2" s="3"/>
+      <c r="K2" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="L2" s="7" t="s">
+      <c r="L2" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="M2" s="5"/>
-      <c r="N2" s="6" t="s">
+      <c r="M2" s="3"/>
+      <c r="N2" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="O2" s="7" t="s">
+      <c r="O2" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="P2" s="5"/>
+      <c r="P2" s="3"/>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A3" s="8"/>
-      <c r="B3" s="9">
+      <c r="A3" s="6"/>
+      <c r="B3" s="7">
         <f>2^1</f>
         <v>2</v>
       </c>
-      <c r="C3" s="10">
+      <c r="C3" s="8">
         <v>9.9999999999999995E-7</v>
       </c>
-      <c r="D3" s="8"/>
-      <c r="E3" s="9">
+      <c r="D3" s="6"/>
+      <c r="E3" s="7">
         <f>2^1</f>
         <v>2</v>
       </c>
-      <c r="F3" s="10">
+      <c r="F3" s="8">
         <v>1.0399999999999999E-4</v>
       </c>
-      <c r="G3" s="8"/>
-      <c r="H3" s="9">
+      <c r="G3" s="6"/>
+      <c r="H3" s="7">
         <f>2^1</f>
         <v>2</v>
       </c>
-      <c r="I3" s="10">
+      <c r="I3" s="8">
         <v>2.2900000000000001E-4</v>
       </c>
-      <c r="J3" s="8"/>
-      <c r="K3" s="9">
+      <c r="J3" s="6"/>
+      <c r="K3" s="7">
         <f>2^1</f>
         <v>2</v>
       </c>
-      <c r="L3" s="10">
+      <c r="L3" s="8">
         <v>2.0699999999999999E-4</v>
       </c>
-      <c r="M3" s="8"/>
-      <c r="N3" s="9">
+      <c r="M3" s="6"/>
+      <c r="N3" s="7">
         <f>2^1</f>
         <v>2</v>
       </c>
-      <c r="O3" s="10">
+      <c r="O3" s="8">
         <v>2.627E-3</v>
       </c>
-      <c r="P3" s="8"/>
+      <c r="P3" s="6"/>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A4" s="11"/>
-      <c r="B4" s="12">
+      <c r="A4" s="9"/>
+      <c r="B4" s="10">
         <f>2^2</f>
         <v>4</v>
       </c>
-      <c r="C4" s="13">
+      <c r="C4" s="11">
         <v>1.0000000000000001E-5</v>
       </c>
-      <c r="D4" s="11"/>
-      <c r="E4" s="12">
+      <c r="D4" s="9"/>
+      <c r="E4" s="10">
         <f>2^2</f>
         <v>4</v>
       </c>
-      <c r="F4" s="13">
+      <c r="F4" s="11">
         <v>1.7100000000000001E-4</v>
       </c>
-      <c r="G4" s="11"/>
-      <c r="H4" s="12">
+      <c r="G4" s="9"/>
+      <c r="H4" s="10">
         <f>2^2</f>
         <v>4</v>
       </c>
-      <c r="I4" s="13">
+      <c r="I4" s="11">
         <v>1.4899999999999999E-4</v>
       </c>
-      <c r="J4" s="11"/>
-      <c r="K4" s="12">
+      <c r="J4" s="9"/>
+      <c r="K4" s="10">
         <f>2^2</f>
         <v>4</v>
       </c>
-      <c r="L4" s="13">
+      <c r="L4" s="11">
         <v>3.1199999999999999E-4</v>
       </c>
-      <c r="M4" s="11"/>
-      <c r="N4" s="12">
+      <c r="M4" s="9"/>
+      <c r="N4" s="10">
         <f>2^2</f>
         <v>4</v>
       </c>
-      <c r="O4" s="13">
+      <c r="O4" s="11">
         <v>4.9880000000000002E-3</v>
       </c>
-      <c r="P4" s="11"/>
+      <c r="P4" s="9"/>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A5" s="11"/>
-      <c r="B5" s="12">
+      <c r="A5" s="9"/>
+      <c r="B5" s="10">
         <f>2^3</f>
         <v>8</v>
       </c>
-      <c r="C5" s="13">
+      <c r="C5" s="11">
         <v>6.0000000000000002E-5</v>
       </c>
-      <c r="D5" s="11"/>
-      <c r="E5" s="12">
+      <c r="D5" s="9"/>
+      <c r="E5" s="10">
         <f>2^3</f>
         <v>8</v>
       </c>
-      <c r="F5" s="13">
+      <c r="F5" s="11">
         <v>1.4799999999999999E-4</v>
       </c>
-      <c r="G5" s="11"/>
-      <c r="H5" s="12">
+      <c r="G5" s="9"/>
+      <c r="H5" s="10">
         <f>2^3</f>
         <v>8</v>
       </c>
-      <c r="I5" s="13">
+      <c r="I5" s="11">
         <v>1.46E-4</v>
       </c>
-      <c r="J5" s="11"/>
-      <c r="K5" s="12">
+      <c r="J5" s="9"/>
+      <c r="K5" s="10">
         <f>2^3</f>
         <v>8</v>
       </c>
-      <c r="L5" s="13">
+      <c r="L5" s="11">
         <v>3.2200000000000002E-4</v>
       </c>
-      <c r="M5" s="11"/>
-      <c r="N5" s="12">
+      <c r="M5" s="9"/>
+      <c r="N5" s="10">
         <f>2^3</f>
         <v>8</v>
       </c>
-      <c r="O5" s="13">
+      <c r="O5" s="11">
         <v>2.591E-3</v>
       </c>
-      <c r="P5" s="11"/>
+      <c r="P5" s="9"/>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A6" s="11"/>
-      <c r="B6" s="12">
+      <c r="A6" s="9"/>
+      <c r="B6" s="10">
         <f>2^4</f>
         <v>16</v>
       </c>
-      <c r="C6" s="13">
+      <c r="C6" s="11">
         <v>1.94E-4</v>
       </c>
-      <c r="D6" s="11"/>
-      <c r="E6" s="12">
+      <c r="D6" s="9"/>
+      <c r="E6" s="10">
         <f>2^4</f>
         <v>16</v>
       </c>
-      <c r="F6" s="13">
+      <c r="F6" s="11">
         <v>1.73E-4</v>
       </c>
-      <c r="G6" s="11"/>
-      <c r="H6" s="12">
+      <c r="G6" s="9"/>
+      <c r="H6" s="10">
         <f>2^4</f>
         <v>16</v>
       </c>
-      <c r="I6" s="13">
+      <c r="I6" s="11">
         <v>1.75E-4</v>
       </c>
-      <c r="J6" s="11"/>
-      <c r="K6" s="12">
+      <c r="J6" s="9"/>
+      <c r="K6" s="10">
         <f>2^4</f>
         <v>16</v>
       </c>
-      <c r="L6" s="13">
+      <c r="L6" s="11">
         <v>2.72E-4</v>
       </c>
-      <c r="M6" s="11"/>
-      <c r="N6" s="12">
+      <c r="M6" s="9"/>
+      <c r="N6" s="10">
         <f>2^4</f>
         <v>16</v>
       </c>
-      <c r="O6" s="13">
+      <c r="O6" s="11">
         <v>2.5850000000000001E-3</v>
       </c>
-      <c r="P6" s="11"/>
+      <c r="P6" s="9"/>
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A7" s="11"/>
-      <c r="B7" s="12">
+      <c r="A7" s="9"/>
+      <c r="B7" s="10">
         <f>2^5</f>
         <v>32</v>
       </c>
-      <c r="C7" s="13">
+      <c r="C7" s="11">
         <v>9.8200000000000002E-4</v>
       </c>
-      <c r="D7" s="11"/>
-      <c r="E7" s="12">
+      <c r="D7" s="9"/>
+      <c r="E7" s="10">
         <f>2^5</f>
         <v>32</v>
       </c>
-      <c r="F7" s="13">
+      <c r="F7" s="11">
         <v>4.2099999999999999E-4</v>
       </c>
-      <c r="G7" s="11"/>
-      <c r="H7" s="12">
+      <c r="G7" s="9"/>
+      <c r="H7" s="10">
         <f>2^5</f>
         <v>32</v>
       </c>
-      <c r="I7" s="13">
+      <c r="I7" s="11">
         <v>3.6099999999999999E-4</v>
       </c>
-      <c r="J7" s="11"/>
-      <c r="K7" s="12">
+      <c r="J7" s="9"/>
+      <c r="K7" s="10">
         <f>2^5</f>
         <v>32</v>
       </c>
-      <c r="L7" s="13">
+      <c r="L7" s="11">
         <v>3.9899999999999999E-4</v>
       </c>
-      <c r="M7" s="11"/>
-      <c r="N7" s="12">
+      <c r="M7" s="9"/>
+      <c r="N7" s="10">
         <f>2^5</f>
         <v>32</v>
       </c>
-      <c r="O7" s="13">
+      <c r="O7" s="11">
         <v>2.9840000000000001E-3</v>
       </c>
-      <c r="P7" s="11"/>
+      <c r="P7" s="9"/>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A8" s="11"/>
-      <c r="B8" s="12">
+      <c r="A8" s="9"/>
+      <c r="B8" s="10">
         <f>2^6</f>
         <v>64</v>
       </c>
-      <c r="C8" s="13">
+      <c r="C8" s="11">
         <v>4.3579999999999999E-3</v>
       </c>
-      <c r="D8" s="11"/>
-      <c r="E8" s="12">
+      <c r="D8" s="9"/>
+      <c r="E8" s="10">
         <f>2^6</f>
         <v>64</v>
       </c>
-      <c r="F8" s="13">
+      <c r="F8" s="11">
         <v>3.5660000000000002E-3</v>
       </c>
-      <c r="G8" s="11"/>
-      <c r="H8" s="12">
+      <c r="G8" s="9"/>
+      <c r="H8" s="10">
         <f>2^6</f>
         <v>64</v>
       </c>
-      <c r="I8" s="13">
+      <c r="I8" s="11">
         <v>3.4090000000000001E-3</v>
       </c>
-      <c r="J8" s="11"/>
-      <c r="K8" s="12">
+      <c r="J8" s="9"/>
+      <c r="K8" s="10">
         <f>2^6</f>
         <v>64</v>
       </c>
-      <c r="L8" s="13">
+      <c r="L8" s="11">
         <v>1.8519999999999999E-3</v>
       </c>
-      <c r="M8" s="11"/>
-      <c r="N8" s="12">
+      <c r="M8" s="9"/>
+      <c r="N8" s="10">
         <f>2^6</f>
         <v>64</v>
       </c>
-      <c r="O8" s="13">
+      <c r="O8" s="11">
         <v>5.7790000000000003E-3</v>
       </c>
-      <c r="P8" s="11"/>
+      <c r="P8" s="9"/>
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A9" s="11"/>
-      <c r="B9" s="12">
+      <c r="A9" s="9"/>
+      <c r="B9" s="10">
         <f>2^7</f>
         <v>128</v>
       </c>
-      <c r="C9" s="13">
+      <c r="C9" s="11">
         <v>2.1871999999999999E-2</v>
       </c>
-      <c r="D9" s="11"/>
-      <c r="E9" s="12">
+      <c r="D9" s="9"/>
+      <c r="E9" s="10">
         <f>2^7</f>
         <v>128</v>
       </c>
-      <c r="F9" s="13">
+      <c r="F9" s="11">
         <v>1.1035E-2</v>
       </c>
-      <c r="G9" s="11"/>
-      <c r="H9" s="12">
+      <c r="G9" s="9"/>
+      <c r="H9" s="10">
         <f>2^7</f>
         <v>128</v>
       </c>
-      <c r="I9" s="13">
+      <c r="I9" s="11">
         <v>1.5179E-2</v>
       </c>
-      <c r="J9" s="11"/>
-      <c r="K9" s="12">
+      <c r="J9" s="9"/>
+      <c r="K9" s="10">
         <f>2^7</f>
         <v>128</v>
       </c>
-      <c r="L9" s="13">
+      <c r="L9" s="11">
         <v>1.3684E-2</v>
       </c>
-      <c r="M9" s="11"/>
-      <c r="N9" s="12">
+      <c r="M9" s="9"/>
+      <c r="N9" s="10">
         <f>2^7</f>
         <v>128</v>
       </c>
-      <c r="O9" s="13">
+      <c r="O9" s="11">
         <v>1.3675E-2</v>
       </c>
-      <c r="P9" s="11"/>
+      <c r="P9" s="9"/>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A10" s="11"/>
-      <c r="B10" s="12">
+      <c r="A10" s="9"/>
+      <c r="B10" s="10">
         <f>2^8</f>
         <v>256</v>
       </c>
-      <c r="C10" s="13">
+      <c r="C10" s="11">
         <v>9.3522999999999995E-2</v>
       </c>
-      <c r="D10" s="11"/>
-      <c r="E10" s="12">
+      <c r="D10" s="9"/>
+      <c r="E10" s="10">
         <f>2^8</f>
         <v>256</v>
       </c>
-      <c r="F10" s="13">
+      <c r="F10" s="11">
         <v>4.0141000000000003E-2</v>
       </c>
-      <c r="G10" s="11"/>
-      <c r="H10" s="12">
+      <c r="G10" s="9"/>
+      <c r="H10" s="10">
         <f>2^8</f>
         <v>256</v>
       </c>
-      <c r="I10" s="13">
+      <c r="I10" s="11">
         <v>2.9731E-2</v>
       </c>
-      <c r="J10" s="11"/>
-      <c r="K10" s="12">
+      <c r="J10" s="9"/>
+      <c r="K10" s="10">
         <f>2^8</f>
         <v>256</v>
       </c>
-      <c r="L10" s="13">
+      <c r="L10" s="11">
         <v>4.743E-2</v>
       </c>
-      <c r="M10" s="11"/>
-      <c r="N10" s="12">
+      <c r="M10" s="9"/>
+      <c r="N10" s="10">
         <f>2^8</f>
         <v>256</v>
       </c>
-      <c r="O10" s="13">
+      <c r="O10" s="11">
         <v>3.6287E-2</v>
       </c>
-      <c r="P10" s="11"/>
+      <c r="P10" s="9"/>
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A11" s="11"/>
-      <c r="B11" s="12">
+      <c r="A11" s="9"/>
+      <c r="B11" s="10">
         <f>2^9</f>
         <v>512</v>
       </c>
-      <c r="C11" s="13">
+      <c r="C11" s="11">
         <v>0.58199100000000004</v>
       </c>
-      <c r="D11" s="11"/>
-      <c r="E11" s="12">
+      <c r="D11" s="9"/>
+      <c r="E11" s="10">
         <f>2^9</f>
         <v>512</v>
       </c>
-      <c r="F11" s="13">
+      <c r="F11" s="11">
         <v>0.15452299999999999</v>
       </c>
-      <c r="G11" s="11"/>
-      <c r="H11" s="12">
+      <c r="G11" s="9"/>
+      <c r="H11" s="10">
         <f>2^9</f>
         <v>512</v>
       </c>
-      <c r="I11" s="13">
+      <c r="I11" s="11">
         <v>0.14475299999999999</v>
       </c>
-      <c r="J11" s="11"/>
-      <c r="K11" s="12">
+      <c r="J11" s="9"/>
+      <c r="K11" s="10">
         <f>2^9</f>
         <v>512</v>
       </c>
-      <c r="L11" s="13">
+      <c r="L11" s="11">
         <v>0.13952000000000001</v>
       </c>
-      <c r="M11" s="11"/>
-      <c r="N11" s="12">
+      <c r="M11" s="9"/>
+      <c r="N11" s="10">
         <f>2^9</f>
         <v>512</v>
       </c>
-      <c r="O11" s="13">
+      <c r="O11" s="11">
         <v>0.153836</v>
       </c>
-      <c r="P11" s="11"/>
+      <c r="P11" s="9"/>
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A12" s="11"/>
-      <c r="B12" s="12">
+      <c r="A12" s="9"/>
+      <c r="B12" s="10">
         <f>2^10</f>
         <v>1024</v>
       </c>
-      <c r="C12" s="13">
+      <c r="C12" s="11">
         <v>5.4001760000000001</v>
       </c>
-      <c r="D12" s="11"/>
-      <c r="E12" s="12">
+      <c r="D12" s="9"/>
+      <c r="E12" s="10">
         <f>2^10</f>
         <v>1024</v>
       </c>
-      <c r="F12" s="13">
+      <c r="F12" s="11">
         <v>2.1780680000000001</v>
       </c>
-      <c r="G12" s="11"/>
-      <c r="H12" s="12">
+      <c r="G12" s="9"/>
+      <c r="H12" s="10">
         <f>2^10</f>
         <v>1024</v>
       </c>
-      <c r="I12" s="13">
+      <c r="I12" s="11">
         <v>2.0929630000000001</v>
       </c>
-      <c r="J12" s="11"/>
-      <c r="K12" s="12">
+      <c r="J12" s="9"/>
+      <c r="K12" s="10">
         <f>2^10</f>
         <v>1024</v>
       </c>
-      <c r="L12" s="13">
+      <c r="L12" s="11">
         <v>2.2452200000000002</v>
       </c>
-      <c r="M12" s="11"/>
-      <c r="N12" s="12">
+      <c r="M12" s="9"/>
+      <c r="N12" s="10">
         <f>2^10</f>
         <v>1024</v>
       </c>
-      <c r="O12" s="13">
+      <c r="O12" s="11">
         <v>1.9982930000000001</v>
       </c>
-      <c r="P12" s="11"/>
+      <c r="P12" s="9"/>
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A13" s="11"/>
-      <c r="B13" s="12">
+      <c r="A13" s="9"/>
+      <c r="B13" s="10">
         <f>2^11</f>
         <v>2048</v>
       </c>
-      <c r="C13" s="13">
+      <c r="C13" s="11">
         <v>106.6818</v>
       </c>
-      <c r="D13" s="11"/>
-      <c r="E13" s="12">
+      <c r="D13" s="9"/>
+      <c r="E13" s="10">
         <f>2^11</f>
         <v>2048</v>
       </c>
-      <c r="F13" s="13">
+      <c r="F13" s="11">
         <v>33.376015000000002</v>
       </c>
-      <c r="G13" s="11"/>
-      <c r="H13" s="12">
+      <c r="G13" s="9"/>
+      <c r="H13" s="10">
         <f>2^11</f>
         <v>2048</v>
       </c>
-      <c r="I13" s="13">
+      <c r="I13" s="11">
         <v>32.353803999999997</v>
       </c>
-      <c r="J13" s="11"/>
-      <c r="K13" s="12">
+      <c r="J13" s="9"/>
+      <c r="K13" s="10">
         <f>2^11</f>
         <v>2048</v>
       </c>
-      <c r="L13" s="13">
+      <c r="L13" s="11">
         <v>32.929046999999997</v>
       </c>
-      <c r="M13" s="11"/>
-      <c r="N13" s="12">
+      <c r="M13" s="9"/>
+      <c r="N13" s="10">
         <f>2^11</f>
         <v>2048</v>
       </c>
-      <c r="O13" s="13">
+      <c r="O13" s="11">
         <v>31.981470000000002</v>
       </c>
-      <c r="P13" s="11"/>
+      <c r="P13" s="9"/>
     </row>
     <row r="14" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="14"/>
-      <c r="B14" s="15">
+      <c r="A14" s="12"/>
+      <c r="B14" s="13">
         <f>2^12</f>
         <v>4096</v>
       </c>
-      <c r="C14" s="16">
+      <c r="C14" s="14">
         <v>918.78635999999995</v>
       </c>
-      <c r="D14" s="14"/>
-      <c r="E14" s="15">
+      <c r="D14" s="12"/>
+      <c r="E14" s="13">
         <f>2^12</f>
         <v>4096</v>
       </c>
-      <c r="F14" s="16">
+      <c r="F14" s="14">
         <v>298.75081399999999</v>
       </c>
-      <c r="G14" s="14"/>
-      <c r="H14" s="15">
+      <c r="G14" s="12"/>
+      <c r="H14" s="13">
         <f>2^12</f>
         <v>4096</v>
       </c>
-      <c r="I14" s="16">
+      <c r="I14" s="14">
         <v>314.23306400000001</v>
       </c>
-      <c r="J14" s="14"/>
-      <c r="K14" s="15">
+      <c r="J14" s="12"/>
+      <c r="K14" s="13">
         <f>2^12</f>
         <v>4096</v>
       </c>
-      <c r="L14" s="16">
+      <c r="L14" s="14">
         <v>319.352711</v>
       </c>
-      <c r="M14" s="14"/>
-      <c r="N14" s="15">
+      <c r="M14" s="12"/>
+      <c r="N14" s="13">
         <f>2^12</f>
         <v>4096</v>
       </c>
-      <c r="O14" s="16">
+      <c r="O14" s="14">
         <v>312.575827</v>
       </c>
-      <c r="P14" s="14"/>
+      <c r="P14" s="12"/>
     </row>
     <row r="15" spans="1:16" ht="9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="17"/>
-      <c r="B15" s="17"/>
-      <c r="C15" s="17"/>
-      <c r="D15" s="17"/>
-      <c r="E15" s="17"/>
-      <c r="F15" s="17"/>
-      <c r="G15" s="17"/>
-      <c r="H15" s="17"/>
-      <c r="I15" s="17"/>
-      <c r="J15" s="17"/>
-      <c r="K15" s="17"/>
-      <c r="L15" s="17"/>
-      <c r="M15" s="17"/>
-      <c r="N15" s="17"/>
-      <c r="O15" s="17"/>
-      <c r="P15" s="17"/>
+      <c r="A15" s="15"/>
+      <c r="B15" s="15"/>
+      <c r="C15" s="15"/>
+      <c r="D15" s="15"/>
+      <c r="E15" s="15"/>
+      <c r="F15" s="15"/>
+      <c r="G15" s="15"/>
+      <c r="H15" s="15"/>
+      <c r="I15" s="15"/>
+      <c r="J15" s="15"/>
+      <c r="K15" s="15"/>
+      <c r="L15" s="15"/>
+      <c r="M15" s="15"/>
+      <c r="N15" s="15"/>
+      <c r="O15" s="15"/>
+      <c r="P15" s="15"/>
     </row>
   </sheetData>
   <mergeCells count="5">

</xml_diff>